<commit_message>
mise a jour UserStorie
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="3"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="107">
   <si>
     <t>priorite</t>
   </si>
@@ -273,12 +273,6 @@
     <t>modification logic pour offrir don pour les champ ajouter</t>
   </si>
   <si>
-    <t>page d'acceuil</t>
-  </si>
-  <si>
-    <t>modification - button, caroussele ?</t>
-  </si>
-  <si>
     <t>traitement de don par employé</t>
   </si>
   <si>
@@ -334,6 +328,21 @@
   </si>
   <si>
     <t>logique CRUD</t>
+  </si>
+  <si>
+    <t>Mise à jour page d'acceuil</t>
+  </si>
+  <si>
+    <t>Mise à jour image catégorie de don</t>
+  </si>
+  <si>
+    <t>Mise à jour barre de navigation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mise à jour connection avec la page connection d' un don </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mise à jour connection avec la page modifier  un don </t>
   </si>
 </sst>
 </file>
@@ -433,14 +442,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -470,9 +473,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -496,6 +496,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -843,7 +855,7 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -851,7 +863,7 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C4">
@@ -862,7 +874,7 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C5">
@@ -873,7 +885,7 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C6">
@@ -884,7 +896,7 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C7">
@@ -1138,13 +1150,13 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="24">
+        <v>1</v>
+      </c>
+      <c r="B2" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="24">
         <v>3</v>
       </c>
       <c r="D2" t="s">
@@ -1155,9 +1167,9 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="2"/>
+      <c r="A3" s="24"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="24"/>
       <c r="D3" t="s">
         <v>34</v>
       </c>
@@ -1166,9 +1178,9 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="2"/>
+      <c r="A4" s="24"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="24"/>
       <c r="D4" t="s">
         <v>36</v>
       </c>
@@ -1177,9 +1189,9 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="2"/>
+      <c r="A5" s="24"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="24"/>
       <c r="D5" t="s">
         <v>38</v>
       </c>
@@ -1188,9 +1200,9 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="2"/>
+      <c r="A6" s="24"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="24"/>
       <c r="D6" t="s">
         <v>40</v>
       </c>
@@ -1199,9 +1211,9 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="2"/>
+      <c r="A7" s="24"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="24"/>
       <c r="D7" t="s">
         <v>41</v>
       </c>
@@ -1210,9 +1222,9 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="2"/>
+      <c r="A8" s="24"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="24"/>
       <c r="D8" t="s">
         <v>42</v>
       </c>
@@ -1221,16 +1233,16 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+      <c r="A9" s="24">
         <v>2</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="24">
         <v>0.5</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="2" t="s">
         <v>45</v>
       </c>
       <c r="F9" t="s">
@@ -1238,9 +1250,9 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="2"/>
+      <c r="A10" s="24"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="24"/>
       <c r="D10" t="s">
         <v>47</v>
       </c>
@@ -1249,16 +1261,16 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+      <c r="A11" s="24">
         <v>3</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="24">
         <v>0.5</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F11" t="s">
@@ -1266,9 +1278,9 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="2"/>
+      <c r="A12" s="24"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="24"/>
       <c r="D12" t="s">
         <v>47</v>
       </c>
@@ -1310,13 +1322,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1378,10 +1390,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1389,525 +1401,573 @@
     <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="59.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="26"/>
+    <col min="5" max="5" width="9.140625" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="10" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:8" s="8" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="G1" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="10">
+        <v>1</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="27"/>
+      <c r="B3" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="10">
+        <v>1</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="27"/>
+      <c r="B4" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="10">
+        <v>1</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="10">
+        <v>1</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="27"/>
+      <c r="B6" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="10">
+        <v>1</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+    </row>
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="27"/>
+      <c r="B7" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="10">
+        <v>1</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="27"/>
+      <c r="B8" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="10">
+        <v>1</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="27"/>
+      <c r="B9" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="10">
+        <v>1</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="27"/>
+      <c r="B10" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="10">
+        <v>1</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="27"/>
+      <c r="B11" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="10">
+        <v>1</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="10">
+        <v>1</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="27"/>
+      <c r="B13" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="10">
+        <v>1</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="10">
+        <v>1</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+    </row>
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="27"/>
+      <c r="B15" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="10">
+        <v>1</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="27"/>
+      <c r="B16" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="10">
+        <v>1</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="10">
+        <v>1</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="10">
+        <v>1</v>
+      </c>
+      <c r="E18" s="21"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="10">
+        <v>1</v>
+      </c>
+      <c r="E19" s="21"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="B20" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="10">
+        <v>1</v>
+      </c>
+      <c r="E20" s="21"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="10">
+        <v>1</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+    </row>
+    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="24"/>
+      <c r="B22" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="10">
+        <v>1</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="24"/>
+      <c r="B23" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" s="10">
+        <v>1</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="24"/>
+      <c r="B24" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" s="10">
+        <v>1</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="24"/>
+      <c r="B25" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" s="10">
+        <v>1</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="E1" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" s="12">
-        <v>1</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="12">
-        <v>1</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" s="12">
-        <v>1</v>
-      </c>
-      <c r="E4" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="C5" s="11" t="s">
+      <c r="B26" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C26" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="12">
-        <v>1</v>
-      </c>
-      <c r="E5" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="C6" s="11" t="s">
+      <c r="D26" s="10">
+        <v>1</v>
+      </c>
+      <c r="E26" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="26"/>
+      <c r="B27" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C27" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="12">
-        <v>1</v>
-      </c>
-      <c r="E6" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-    </row>
-    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="12">
-        <v>1</v>
-      </c>
-      <c r="E7" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" s="12">
-        <v>1</v>
-      </c>
-      <c r="E8" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="12">
-        <v>1</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="12">
-        <v>1</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11" s="12">
-        <v>1</v>
-      </c>
-      <c r="E11" s="22" t="s">
-        <v>95</v>
-      </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-    </row>
-    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="D12" s="12">
-        <v>1</v>
-      </c>
-      <c r="E12" s="23" t="s">
-        <v>95</v>
-      </c>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="D13" s="12">
-        <v>1</v>
-      </c>
-      <c r="E13" s="23" t="s">
-        <v>95</v>
-      </c>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" s="12">
-        <v>1</v>
-      </c>
-      <c r="E14" s="23" t="s">
-        <v>95</v>
-      </c>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-    </row>
-    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="D15" s="12">
-        <v>1</v>
-      </c>
-      <c r="E15" s="23" t="s">
-        <v>95</v>
-      </c>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
-      <c r="B16" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="D16" s="12">
-        <v>1</v>
-      </c>
-      <c r="E16" s="23" t="s">
-        <v>95</v>
-      </c>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="12">
-        <v>1</v>
-      </c>
-      <c r="E17" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" s="12">
-        <v>1</v>
-      </c>
-      <c r="E18" s="22" t="s">
-        <v>95</v>
-      </c>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-    </row>
-    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D19" s="12">
-        <v>1</v>
-      </c>
-      <c r="E19" s="22" t="s">
-        <v>95</v>
-      </c>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D20" s="12">
-        <v>1</v>
-      </c>
-      <c r="E20" s="22" t="s">
-        <v>95</v>
-      </c>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D21" s="12">
-        <v>1</v>
-      </c>
-      <c r="E21" s="22" t="s">
-        <v>95</v>
-      </c>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D22" s="12">
-        <v>1</v>
-      </c>
-      <c r="E22" s="22" t="s">
-        <v>95</v>
-      </c>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="B23" s="11" t="s">
+      <c r="D27" s="10">
+        <v>1</v>
+      </c>
+      <c r="E27" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="26"/>
+      <c r="B28" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C28" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="12">
-        <v>1</v>
-      </c>
-      <c r="E23" s="25" t="s">
-        <v>95</v>
-      </c>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="18"/>
-      <c r="B24" s="11" t="s">
+      <c r="D28" s="10">
+        <v>1</v>
+      </c>
+      <c r="E28" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="26"/>
+      <c r="B29" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C29" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D24" s="12">
-        <v>1</v>
-      </c>
-      <c r="E24" s="25" t="s">
-        <v>95</v>
-      </c>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="18"/>
-      <c r="B25" s="11" t="s">
+      <c r="D29" s="10">
+        <v>1</v>
+      </c>
+      <c r="E29" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="26"/>
+      <c r="B30" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C30" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="12">
-        <v>1</v>
-      </c>
-      <c r="E25" s="25" t="s">
-        <v>95</v>
-      </c>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="18"/>
-      <c r="B26" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26" s="12">
-        <v>1</v>
-      </c>
-      <c r="E26" s="25" t="s">
-        <v>95</v>
-      </c>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="18"/>
-      <c r="B27" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D27" s="12">
-        <v>1</v>
-      </c>
-      <c r="E27" s="25" t="s">
-        <v>95</v>
-      </c>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
+      <c r="D30" s="10">
+        <v>1</v>
+      </c>
+      <c r="E30" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A26:A30"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:A11"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A18:A22"/>
-    <mergeCell ref="A23:A27"/>
+    <mergeCell ref="A21:A25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Ajout AfficherDonEmploye.php, traiterDon.php, modification 6-LesDon.class.php, DonsDAO.class.php, Controle_Login.php, userstories.xlsx
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="103">
   <si>
     <t xml:space="preserve">priorite</t>
   </si>
@@ -247,28 +247,28 @@
     <t xml:space="preserve">table organisme et relation avec membre</t>
   </si>
   <si>
-    <t xml:space="preserve">ajout dans la logique promesse don(methodes)</t>
+    <t xml:space="preserve">ajout dans la logique promesse don(méthodes)</t>
   </si>
   <si>
     <t xml:space="preserve">promesse don</t>
   </si>
   <si>
-    <t xml:space="preserve">form validation(etoiles, message d'erreur, formulaire vide)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">modal redirection après promesse don reusi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mode de livraison interface, modification logique pour offrir don(2 radio butoons et leur desactivation si argent)</t>
+    <t xml:space="preserve">form validation(étoiles, message d'erreur, formulaire vide)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">modal redirection après promesse don reçu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mode de livraison interface, modification logique pour offrir don(2 radio butons et leur désactivation si argent)</t>
   </si>
   <si>
     <t xml:space="preserve">ajout des ville, province, code postal dans l'interface</t>
   </si>
   <si>
-    <t xml:space="preserve">modification dans la table concernant l'adress</t>
-  </si>
-  <si>
-    <t xml:space="preserve">modification logic pour offrir don pour les champ ajouter</t>
+    <t xml:space="preserve">modification dans la table concernant l'adresse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">modification logique pour offrir don pour les champ ajouter</t>
   </si>
   <si>
     <t xml:space="preserve">mis a jour des données de membre si un donateur existant</t>
@@ -277,7 +277,7 @@
     <t xml:space="preserve">annuler</t>
   </si>
   <si>
-    <t xml:space="preserve">interface - liste des dons qui sont pas traités(nom, quantite, categorie, montant, mode livraison, date promise)</t>
+    <t xml:space="preserve">interface - liste des dons qui sont pas traités(nom, quantité, catégorie, montant, mode livraison, date promise)</t>
   </si>
   <si>
     <t xml:space="preserve">logique pour annuler </t>
@@ -295,10 +295,7 @@
     <t xml:space="preserve">ajout logique modifier</t>
   </si>
   <si>
-    <t xml:space="preserve">page d'acceuil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">modification - button, caroussele ?</t>
+    <t xml:space="preserve">modification – button, caroussele ?</t>
   </si>
   <si>
     <t xml:space="preserve">traitement de don par employé</t>
@@ -313,16 +310,16 @@
     <t xml:space="preserve">envoie courriel au donateur</t>
   </si>
   <si>
-    <t xml:space="preserve">envoier courriel a partir de lien modifier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">se autrhetifier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">propose se diponibilité comme benevole</t>
-  </si>
-  <si>
-    <t xml:space="preserve">buton nav pour formulaire</t>
+    <t xml:space="preserve">envoie courriel a partir de lien modifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">se authentifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">propose se disponibilité comme bénévole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">button nav pour formulaire</t>
   </si>
   <si>
     <t xml:space="preserve">formulaire pour disponibilité</t>
@@ -331,7 +328,7 @@
     <t xml:space="preserve">table dans la base</t>
   </si>
   <si>
-    <t xml:space="preserve">class, DAO</t>
+    <t xml:space="preserve">classe, DAO</t>
   </si>
   <si>
     <t xml:space="preserve">logique CRUD</t>
@@ -652,7 +649,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="117.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.71"/>
   </cols>
   <sheetData>
@@ -954,10 +951,10 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="44.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="40.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="8.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.71"/>
   </cols>
   <sheetData>
@@ -1161,7 +1158,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="81.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="70.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.67"/>
   </cols>
   <sheetData>
@@ -1240,17 +1237,17 @@
   </sheetPr>
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="59.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="6" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="6" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.67"/>
   </cols>
   <sheetData>
@@ -1374,7 +1371,7 @@
       <c r="G6" s="13"/>
       <c r="H6" s="13"/>
     </row>
-    <row r="7" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10"/>
       <c r="B7" s="15" t="s">
         <v>78</v>
@@ -1464,7 +1461,7 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="10" t="s">
         <v>83</v>
       </c>
@@ -1560,10 +1557,10 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="21" t="s">
         <v>90</v>
-      </c>
-      <c r="B17" s="21" t="s">
-        <v>91</v>
       </c>
       <c r="C17" s="21" t="s">
         <v>37</v>
@@ -1580,10 +1577,10 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>43</v>
@@ -1601,7 +1598,7 @@
     <row r="19" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="10"/>
       <c r="B19" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>43</v>
@@ -1619,7 +1616,7 @@
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="10"/>
       <c r="B20" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>43</v>
@@ -1637,7 +1634,7 @@
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="10"/>
       <c r="B21" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>43</v>
@@ -1655,7 +1652,7 @@
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="10"/>
       <c r="B22" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>43</v>
@@ -1672,10 +1669,10 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="B23" s="13" t="s">
         <v>98</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>99</v>
       </c>
       <c r="C23" s="13" t="s">
         <v>33</v>
@@ -1693,7 +1690,7 @@
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="24"/>
       <c r="B24" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C24" s="13" t="s">
         <v>33</v>
@@ -1711,7 +1708,7 @@
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="24"/>
       <c r="B25" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C25" s="13" t="s">
         <v>33</v>
@@ -1729,7 +1726,7 @@
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="24"/>
       <c r="B26" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C26" s="13" t="s">
         <v>33</v>
@@ -1747,7 +1744,7 @@
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="24"/>
       <c r="B27" s="13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C27" s="13" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
Ajout de fonctionallites accepter et refuser don avec envoie d'un courriel
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -649,7 +649,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="117.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.71"/>
   </cols>
   <sheetData>
@@ -951,7 +951,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="44.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="40.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="8.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.3"/>
@@ -1238,14 +1238,14 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
+      <selection pane="topLeft" activeCell="J17" activeCellId="0" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="59.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="6" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.67"/>
@@ -1575,7 +1575,7 @@
       <c r="G17" s="21"/>
       <c r="H17" s="21"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="10" t="s">
         <v>91</v>
       </c>
@@ -1588,14 +1588,14 @@
       <c r="D18" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="E18" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="F18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="16" t="s">
+        <v>72</v>
+      </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="10"/>
       <c r="B19" s="23" t="s">
         <v>93</v>
@@ -1606,14 +1606,14 @@
       <c r="D19" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="E19" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="F19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="16" t="s">
+        <v>72</v>
+      </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="10"/>
       <c r="B20" s="1" t="s">
         <v>94</v>
@@ -1624,10 +1624,10 @@
       <c r="D20" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="E20" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="F20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="16" t="s">
+        <v>72</v>
+      </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
     </row>

</xml_diff>

<commit_message>
modification fichier excel userStory
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="113">
   <si>
     <t>priorite</t>
   </si>
@@ -343,6 +343,24 @@
   </si>
   <si>
     <t xml:space="preserve">Mise à jour connection avec la page modifier  un don </t>
+  </si>
+  <si>
+    <t>Gestion Bénévole</t>
+  </si>
+  <si>
+    <t>Ajout des liens pour la modification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Afficher la liste des Bénévoles </t>
+  </si>
+  <si>
+    <t>Créer un lien pour permettre au Bénévole de modifier</t>
+  </si>
+  <si>
+    <t>son adresse et son courriel</t>
+  </si>
+  <si>
+    <t>Créer un lien pour permettre au Bénévole de désactiver</t>
   </si>
 </sst>
 </file>
@@ -442,7 +460,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -450,12 +468,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -497,6 +509,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -509,6 +524,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -885,7 +904,7 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C6">
@@ -896,7 +915,7 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C7">
@@ -1150,13 +1169,13 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="24">
-        <v>1</v>
-      </c>
-      <c r="B2" s="25" t="s">
+      <c r="A2" s="23">
+        <v>1</v>
+      </c>
+      <c r="B2" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="24">
+      <c r="C2" s="23">
         <v>3</v>
       </c>
       <c r="D2" t="s">
@@ -1167,9 +1186,9 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="24"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="24"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="23"/>
       <c r="D3" t="s">
         <v>34</v>
       </c>
@@ -1178,9 +1197,9 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="24"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="23"/>
       <c r="D4" t="s">
         <v>36</v>
       </c>
@@ -1189,9 +1208,9 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="24"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="23"/>
       <c r="D5" t="s">
         <v>38</v>
       </c>
@@ -1200,9 +1219,9 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="24"/>
+      <c r="A6" s="23"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="23"/>
       <c r="D6" t="s">
         <v>40</v>
       </c>
@@ -1211,9 +1230,9 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="24"/>
+      <c r="A7" s="23"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="23"/>
       <c r="D7" t="s">
         <v>41</v>
       </c>
@@ -1222,9 +1241,9 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="24"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="24"/>
+      <c r="A8" s="23"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="23"/>
       <c r="D8" t="s">
         <v>42</v>
       </c>
@@ -1233,13 +1252,13 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="24">
+      <c r="A9" s="23">
         <v>2</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="24">
+      <c r="C9" s="23">
         <v>0.5</v>
       </c>
       <c r="D9" s="2" t="s">
@@ -1250,9 +1269,9 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="24"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="24"/>
+      <c r="A10" s="23"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="23"/>
       <c r="D10" t="s">
         <v>47</v>
       </c>
@@ -1261,13 +1280,13 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="24">
+      <c r="A11" s="23">
         <v>3</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="24">
+      <c r="C11" s="23">
         <v>0.5</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -1278,9 +1297,9 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="24"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="24"/>
+      <c r="A12" s="23"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="23"/>
       <c r="D12" t="s">
         <v>47</v>
       </c>
@@ -1390,10 +1409,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1401,573 +1420,675 @@
     <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="59.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="23"/>
+    <col min="5" max="5" width="9.140625" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="8" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:8" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="5" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="10">
-        <v>1</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
+      <c r="D2" s="8">
+        <v>1</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="27"/>
-      <c r="B3" s="10" t="s">
+      <c r="A3" s="26"/>
+      <c r="B3" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="10">
-        <v>1</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
+      <c r="D3" s="8">
+        <v>1</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="27"/>
-      <c r="B4" s="10" t="s">
+      <c r="A4" s="26"/>
+      <c r="B4" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="10">
-        <v>1</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
+      <c r="D4" s="8">
+        <v>1</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="10">
-        <v>1</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
+      <c r="D5" s="8">
+        <v>1</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="27"/>
-      <c r="B6" s="9" t="s">
+      <c r="A6" s="26"/>
+      <c r="B6" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="10">
-        <v>1</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
+      <c r="D6" s="8">
+        <v>1</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
-      <c r="B7" s="11" t="s">
+      <c r="A7" s="26"/>
+      <c r="B7" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="10">
-        <v>1</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
+      <c r="D7" s="8">
+        <v>1</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
-      <c r="B8" s="10" t="s">
+      <c r="A8" s="26"/>
+      <c r="B8" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="10">
-        <v>1</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
+      <c r="D8" s="8">
+        <v>1</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="27"/>
-      <c r="B9" s="10" t="s">
+      <c r="A9" s="26"/>
+      <c r="B9" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="10">
-        <v>1</v>
-      </c>
-      <c r="E9" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
+      <c r="D9" s="8">
+        <v>1</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="27"/>
-      <c r="B10" s="10" t="s">
+      <c r="A10" s="26"/>
+      <c r="B10" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="10">
-        <v>1</v>
-      </c>
-      <c r="E10" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
+      <c r="D10" s="8">
+        <v>1</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="27"/>
-      <c r="B11" s="6" t="s">
+      <c r="A11" s="26"/>
+      <c r="B11" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="10">
-        <v>1</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
+      <c r="D11" s="8">
+        <v>1</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="10">
-        <v>1</v>
-      </c>
-      <c r="E12" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
+      <c r="D12" s="8">
+        <v>1</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
-      <c r="B13" s="13" t="s">
+      <c r="A13" s="26"/>
+      <c r="B13" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="10">
-        <v>1</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
+      <c r="D13" s="8">
+        <v>1</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="10">
-        <v>1</v>
-      </c>
-      <c r="E14" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
+      <c r="D14" s="8">
+        <v>1</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
     </row>
     <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="27"/>
-      <c r="B15" s="12" t="s">
+      <c r="A15" s="26"/>
+      <c r="B15" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="10">
-        <v>1</v>
-      </c>
-      <c r="E15" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
+      <c r="D15" s="8">
+        <v>1</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="27"/>
-      <c r="B16" s="13" t="s">
+      <c r="A16" s="26"/>
+      <c r="B16" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="D16" s="10">
-        <v>1</v>
-      </c>
-      <c r="E16" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
+      <c r="D16" s="8">
+        <v>1</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="10">
-        <v>1</v>
-      </c>
-      <c r="E17" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
+      <c r="D17" s="8">
+        <v>1</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="15" t="s">
+      <c r="A18" s="26"/>
+      <c r="B18" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="10">
-        <v>1</v>
-      </c>
-      <c r="E18" s="21"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
+      <c r="D18" s="8">
+        <v>1</v>
+      </c>
+      <c r="E18" s="19"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="15" t="s">
+      <c r="A19" s="26"/>
+      <c r="B19" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="10">
-        <v>1</v>
-      </c>
-      <c r="E19" s="21"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
+      <c r="D19" s="8">
+        <v>1</v>
+      </c>
+      <c r="E19" s="19"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="15" t="s">
+      <c r="A20" s="26"/>
+      <c r="B20" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="13"/>
+      <c r="D20" s="8">
+        <v>1</v>
+      </c>
+      <c r="E20" s="19"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="26"/>
+      <c r="B21" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C21" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="10">
-        <v>1</v>
-      </c>
-      <c r="E20" s="21"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="24" t="s">
+      <c r="D21" s="8">
+        <v>1</v>
+      </c>
+      <c r="E21" s="19"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="22"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="8">
+        <v>1</v>
+      </c>
+      <c r="E22" s="19"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="8">
+        <v>1</v>
+      </c>
+      <c r="E23" s="19"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="28"/>
+      <c r="B24" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" s="8">
+        <v>1</v>
+      </c>
+      <c r="E24" s="19"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="28"/>
+      <c r="B25" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="C25" s="13"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="28"/>
+      <c r="B26" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="8">
+        <v>1</v>
+      </c>
+      <c r="E26" s="19"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="28"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B28" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C28" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D21" s="10">
-        <v>1</v>
-      </c>
-      <c r="E21" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-    </row>
-    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="24"/>
-      <c r="B22" s="14" t="s">
+      <c r="D28" s="8">
+        <v>1</v>
+      </c>
+      <c r="E28" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+    </row>
+    <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="23"/>
+      <c r="B29" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C29" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D22" s="10">
-        <v>1</v>
-      </c>
-      <c r="E22" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="24"/>
-      <c r="B23" s="6" t="s">
+      <c r="D29" s="8">
+        <v>1</v>
+      </c>
+      <c r="E29" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="23"/>
+      <c r="B30" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C30" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="10">
-        <v>1</v>
-      </c>
-      <c r="E23" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="24"/>
-      <c r="B24" s="6" t="s">
+      <c r="D30" s="8">
+        <v>1</v>
+      </c>
+      <c r="E30" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="23"/>
+      <c r="B31" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C31" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D24" s="10">
-        <v>1</v>
-      </c>
-      <c r="E24" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="24"/>
-      <c r="B25" s="6" t="s">
+      <c r="D31" s="8">
+        <v>1</v>
+      </c>
+      <c r="E31" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="23"/>
+      <c r="B32" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C32" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="10">
-        <v>1</v>
-      </c>
-      <c r="E25" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="26" t="s">
+      <c r="D32" s="8">
+        <v>1</v>
+      </c>
+      <c r="E32" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B33" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C33" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D26" s="10">
-        <v>1</v>
-      </c>
-      <c r="E26" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="26"/>
-      <c r="B27" s="9" t="s">
+      <c r="D33" s="8">
+        <v>1</v>
+      </c>
+      <c r="E33" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="25"/>
+      <c r="B34" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C34" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D27" s="10">
-        <v>1</v>
-      </c>
-      <c r="E27" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="26"/>
-      <c r="B28" s="9" t="s">
+      <c r="D34" s="8">
+        <v>1</v>
+      </c>
+      <c r="E34" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="25"/>
+      <c r="B35" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C35" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="10">
-        <v>1</v>
-      </c>
-      <c r="E28" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="26"/>
-      <c r="B29" s="9" t="s">
+      <c r="D35" s="8">
+        <v>1</v>
+      </c>
+      <c r="E35" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="25"/>
+      <c r="B36" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="C36" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D29" s="10">
-        <v>1</v>
-      </c>
-      <c r="E29" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="26"/>
-      <c r="B30" s="9" t="s">
+      <c r="D36" s="8">
+        <v>1</v>
+      </c>
+      <c r="E36" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="25"/>
+      <c r="B37" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="C37" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D30" s="10">
-        <v>1</v>
-      </c>
-      <c r="E30" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
+      <c r="D37" s="8">
+        <v>1</v>
+      </c>
+      <c r="E37" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A26:A30"/>
+  <mergeCells count="8">
+    <mergeCell ref="A23:A27"/>
+    <mergeCell ref="A33:A37"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:A11"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="A28:A32"/>
+    <mergeCell ref="A17:A21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Guy logiDon mise à jour terminé
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="113">
   <si>
     <t>priorite</t>
   </si>
@@ -339,9 +339,6 @@
     <t>Mise à jour barre de navigation</t>
   </si>
   <si>
-    <t xml:space="preserve">Mise à jour connection avec la page connection d' un don </t>
-  </si>
-  <si>
     <t xml:space="preserve">Mise à jour connection avec la page modifier  un don </t>
   </si>
   <si>
@@ -351,13 +348,19 @@
     <t>Gestion Bénévole</t>
   </si>
   <si>
-    <t>Afficher les dons attribuer au benevole</t>
-  </si>
-  <si>
-    <t>Modifier son adresse et son courriel</t>
-  </si>
-  <si>
     <t>Créer un lien pour permettre au Bénévole de désactiver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mise à jour connection avec la page faire  un don </t>
+  </si>
+  <si>
+    <t>Afficher les informations sur le benevole après connexion</t>
+  </si>
+  <si>
+    <t>Créer un lien pour permettre au Bénévole de modifier les infos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> telles que:adresse, ville, province,code postale,téléphone</t>
   </si>
 </sst>
 </file>
@@ -461,18 +464,6 @@
   </cellStyleXfs>
   <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -512,9 +503,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -523,8 +511,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -936,7 +939,7 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -944,7 +947,7 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C4">
@@ -955,7 +958,7 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C5">
@@ -966,7 +969,7 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C6">
@@ -977,7 +980,7 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C7">
@@ -988,7 +991,7 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C8">
@@ -999,7 +1002,7 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C9">
@@ -1231,13 +1234,13 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="23">
+        <v>1</v>
+      </c>
+      <c r="B2" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="23">
         <v>3</v>
       </c>
       <c r="D2" t="s">
@@ -1248,9 +1251,9 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="4"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="23"/>
       <c r="D3" t="s">
         <v>34</v>
       </c>
@@ -1259,9 +1262,9 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="4"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="23"/>
       <c r="D4" t="s">
         <v>36</v>
       </c>
@@ -1270,9 +1273,9 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="4"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="23"/>
       <c r="D5" t="s">
         <v>38</v>
       </c>
@@ -1281,9 +1284,9 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="4"/>
+      <c r="A6" s="23"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="23"/>
       <c r="D6" t="s">
         <v>40</v>
       </c>
@@ -1292,9 +1295,9 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="4"/>
+      <c r="A7" s="23"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="23"/>
       <c r="D7" t="s">
         <v>41</v>
       </c>
@@ -1303,9 +1306,9 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="4"/>
+      <c r="A8" s="23"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="23"/>
       <c r="D8" t="s">
         <v>42</v>
       </c>
@@ -1314,16 +1317,16 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="A9" s="23">
         <v>2</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="23">
         <v>0.5</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="2" t="s">
         <v>45</v>
       </c>
       <c r="F9" t="s">
@@ -1331,9 +1334,9 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="4"/>
+      <c r="A10" s="23"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="23"/>
       <c r="D10" t="s">
         <v>47</v>
       </c>
@@ -1342,16 +1345,16 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+      <c r="A11" s="23">
         <v>3</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="23">
         <v>0.5</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F11" t="s">
@@ -1359,9 +1362,9 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="4"/>
+      <c r="A12" s="23"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="23"/>
       <c r="D12" t="s">
         <v>47</v>
       </c>
@@ -1404,13 +1407,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="3" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1474,8 +1477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1484,663 +1487,665 @@
     <col min="2" max="2" width="59.85546875" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="4" customWidth="1"/>
     <col min="6" max="1025" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="11" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:8" s="7" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="5" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="12">
-        <v>1</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
+      <c r="D2" s="8">
+        <v>1</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="12" t="s">
+      <c r="A3" s="28"/>
+      <c r="B3" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="12">
-        <v>1</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
+      <c r="D3" s="8">
+        <v>1</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="12" t="s">
+      <c r="A4" s="28"/>
+      <c r="B4" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="12">
-        <v>1</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
+      <c r="D4" s="8">
+        <v>1</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="12">
-        <v>1</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
+      <c r="D5" s="8">
+        <v>1</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="14" t="s">
+      <c r="A6" s="28"/>
+      <c r="B6" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="12">
-        <v>1</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
+      <c r="D6" s="8">
+        <v>1</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
     </row>
     <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="16" t="s">
+      <c r="A7" s="28"/>
+      <c r="B7" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="12">
-        <v>1</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
+      <c r="D7" s="8">
+        <v>1</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="12" t="s">
+      <c r="A8" s="28"/>
+      <c r="B8" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="12">
-        <v>1</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
+      <c r="D8" s="8">
+        <v>1</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="12" t="s">
+      <c r="A9" s="28"/>
+      <c r="B9" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="12">
-        <v>1</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
+      <c r="D9" s="8">
+        <v>1</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="12" t="s">
+      <c r="A10" s="28"/>
+      <c r="B10" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="12">
-        <v>1</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
+      <c r="D10" s="8">
+        <v>1</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="5" t="s">
+      <c r="A11" s="28"/>
+      <c r="B11" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="12">
-        <v>1</v>
-      </c>
-      <c r="E11" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
+      <c r="D11" s="8">
+        <v>1</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="12">
-        <v>1</v>
-      </c>
-      <c r="E12" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
+      <c r="D12" s="8">
+        <v>1</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="19" t="s">
+      <c r="A13" s="28"/>
+      <c r="B13" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="12">
-        <v>1</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
+      <c r="D13" s="8">
+        <v>1</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="12">
-        <v>1</v>
-      </c>
-      <c r="E14" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
+      <c r="D14" s="8">
+        <v>1</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
     </row>
     <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="18" t="s">
+      <c r="A15" s="28"/>
+      <c r="B15" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="12">
-        <v>1</v>
-      </c>
-      <c r="E15" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
+      <c r="D15" s="8">
+        <v>1</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="19" t="s">
+      <c r="A16" s="28"/>
+      <c r="B16" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="D16" s="12">
-        <v>1</v>
-      </c>
-      <c r="E16" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
+      <c r="D16" s="8">
+        <v>1</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D17" s="12">
-        <v>1</v>
-      </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
+      <c r="D17" s="8">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="21" t="s">
+      <c r="A18" s="28"/>
+      <c r="B18" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D18" s="12">
-        <v>1</v>
-      </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
+      <c r="D18" s="8">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="5" t="s">
+      <c r="A19" s="28"/>
+      <c r="B19" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="12">
-        <v>1</v>
-      </c>
-      <c r="E19" s="5"/>
-      <c r="F19" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
+      <c r="D19" s="8">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="5" t="s">
+      <c r="A20" s="28"/>
+      <c r="B20" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="12">
-        <v>1</v>
-      </c>
-      <c r="E20" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
+      <c r="D20" s="8">
+        <v>1</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="5" t="s">
+      <c r="A21" s="28"/>
+      <c r="B21" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D21" s="12">
-        <v>1</v>
-      </c>
-      <c r="E21" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
+      <c r="D21" s="8">
+        <v>1</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
     </row>
     <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="12">
-        <v>1</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
+      <c r="D22" s="8">
+        <v>1</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="14" t="s">
+      <c r="A23" s="25"/>
+      <c r="B23" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="12">
-        <v>1</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
+      <c r="D23" s="8">
+        <v>1</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="14" t="s">
+      <c r="A24" s="25"/>
+      <c r="B24" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D24" s="12">
-        <v>1</v>
-      </c>
-      <c r="E24" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
+      <c r="D24" s="8">
+        <v>1</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="14" t="s">
+      <c r="A25" s="25"/>
+      <c r="B25" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="12">
-        <v>1</v>
-      </c>
-      <c r="E25" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
+      <c r="D25" s="8">
+        <v>1</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="14" t="s">
+      <c r="A26" s="25"/>
+      <c r="B26" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D26" s="12">
-        <v>1</v>
-      </c>
-      <c r="E26" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
+      <c r="D26" s="8">
+        <v>1</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="22" t="s">
+      <c r="A27" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="B27" s="23" t="s">
+      <c r="B27" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="C27" s="23" t="s">
+      <c r="C27" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="D27" s="24">
-        <v>1</v>
-      </c>
-      <c r="E27" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="F27" s="23"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="23"/>
+      <c r="D27" s="19">
+        <v>1</v>
+      </c>
+      <c r="E27" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="22"/>
-      <c r="B28" s="23" t="s">
+      <c r="A28" s="26"/>
+      <c r="B28" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="C28" s="23" t="s">
+      <c r="C28" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="D28" s="24">
-        <v>1</v>
-      </c>
-      <c r="E28" s="25"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="23"/>
+      <c r="D28" s="19">
+        <v>1</v>
+      </c>
+      <c r="E28" s="20"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="22"/>
-      <c r="B29" s="23" t="s">
+      <c r="A29" s="26"/>
+      <c r="B29" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29" s="19">
+        <v>1</v>
+      </c>
+      <c r="E29" s="20"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="18"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="26"/>
+      <c r="B30" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="C29" s="23" t="s">
+      <c r="C30" s="18"/>
+      <c r="D30" s="19">
+        <v>1</v>
+      </c>
+      <c r="E30" s="20"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="18"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="26"/>
+      <c r="B31" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="C31" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="D29" s="24">
-        <v>1</v>
-      </c>
-      <c r="E29" s="25"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="23"/>
-      <c r="H29" s="23"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="22"/>
-      <c r="B30" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="C30" s="23"/>
-      <c r="D30" s="24">
-        <v>1</v>
-      </c>
-      <c r="E30" s="25"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="23"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="22"/>
-      <c r="B31" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="C31" s="23" t="s">
+      <c r="D31" s="19">
+        <v>1</v>
+      </c>
+      <c r="E31" s="20"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="18"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="21"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="D31" s="24">
-        <v>1</v>
-      </c>
-      <c r="E31" s="25"/>
-      <c r="F31" s="23"/>
-      <c r="G31" s="23"/>
-      <c r="H31" s="23"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="26"/>
-      <c r="B32" s="23"/>
-      <c r="C32" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="D32" s="24">
-        <v>1</v>
-      </c>
-      <c r="E32" s="25"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="23"/>
-      <c r="H32" s="23"/>
+      <c r="D32" s="19">
+        <v>1</v>
+      </c>
+      <c r="E32" s="20"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="B33" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="C33" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="B33" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="C33" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="D33" s="24">
-        <v>1</v>
-      </c>
-      <c r="E33" s="25"/>
-      <c r="F33" s="23"/>
-      <c r="G33" s="23"/>
-      <c r="H33" s="23"/>
+      <c r="D33" s="19">
+        <v>1</v>
+      </c>
+      <c r="E33" s="20"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="18"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="27"/>
-      <c r="B34" s="28"/>
-      <c r="C34" s="23" t="s">
+      <c r="B34" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="C34" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="D34" s="24">
-        <v>1</v>
-      </c>
-      <c r="E34" s="25"/>
-      <c r="F34" s="23"/>
-      <c r="G34" s="23"/>
-      <c r="H34" s="23"/>
+      <c r="D34" s="19">
+        <v>1</v>
+      </c>
+      <c r="E34" s="20"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="18"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="27"/>
-      <c r="B35" s="28" t="s">
-        <v>110</v>
-      </c>
-      <c r="C35" s="23"/>
-      <c r="D35" s="24"/>
-      <c r="E35" s="25"/>
-      <c r="F35" s="23"/>
-      <c r="G35" s="23"/>
-      <c r="H35" s="23"/>
+      <c r="B35" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="C35" s="18"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="18"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="27"/>
-      <c r="B36" s="28" t="s">
-        <v>111</v>
-      </c>
-      <c r="C36" s="23" t="s">
+      <c r="B36" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="C36" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="D36" s="24">
-        <v>1</v>
-      </c>
-      <c r="E36" s="25"/>
-      <c r="F36" s="23"/>
-      <c r="G36" s="23"/>
-      <c r="H36" s="23"/>
+      <c r="D36" s="19">
+        <v>1</v>
+      </c>
+      <c r="E36" s="20"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="27"/>
-      <c r="B37" s="28"/>
-      <c r="C37" s="23"/>
-      <c r="D37" s="24"/>
-      <c r="E37" s="25"/>
-      <c r="F37" s="23"/>
-      <c r="G37" s="23"/>
-      <c r="H37" s="23"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
+      <c r="H37" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>